<commit_message>
Layout edited.  ASSIGNMENT COMPLEEEEEEEETE.
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="20730" windowHeight="10035"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="50">
   <si>
     <t>X</t>
   </si>
@@ -142,13 +142,37 @@
   </si>
   <si>
     <t>Doors</t>
+  </si>
+  <si>
+    <t>Edge Adjacency Test</t>
+  </si>
+  <si>
+    <t>Walkway Adjacency Test</t>
+  </si>
+  <si>
+    <t>Non-Doorway Adjacency Test</t>
+  </si>
+  <si>
+    <t>Next-to-Doorway Adjacency Test</t>
+  </si>
+  <si>
+    <t>Adjacency Test from Doorway.</t>
+  </si>
+  <si>
+    <t>Walkway Target Test</t>
+  </si>
+  <si>
+    <t>Can-Target-Door Test</t>
+  </si>
+  <si>
+    <t>From Doorway Target Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +194,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +230,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -376,7 +455,62 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -680,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +948,7 @@
       <c r="L2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="32" t="s">
         <v>23</v>
       </c>
       <c r="N2" s="14" t="s">
@@ -885,7 +1019,7 @@
       <c r="F3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="28" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -912,13 +1046,13 @@
       <c r="O3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="28" t="s">
         <v>23</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="47" t="s">
         <v>23</v>
       </c>
       <c r="S3" s="8" t="s">
@@ -1029,7 +1163,7 @@
         <v>20</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Z4" s="17" t="s">
         <v>20</v>
@@ -1493,7 +1627,7 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -1511,13 +1645,13 @@
       <c r="G10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="39" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="47" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="8" t="s">
@@ -1544,7 +1678,7 @@
       <c r="R10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="36" t="s">
         <v>23</v>
       </c>
       <c r="T10" s="16" t="s">
@@ -1582,7 +1716,7 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="46" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1740,7 +1874,7 @@
       <c r="X12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="Y12" s="10" t="s">
+      <c r="Y12" s="51" t="s">
         <v>33</v>
       </c>
       <c r="Z12" s="24" t="s">
@@ -1829,10 +1963,10 @@
       <c r="X13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z13" s="18" t="s">
+      <c r="Y13" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z13" s="33" t="s">
         <v>23</v>
       </c>
       <c r="AA13" s="2">
@@ -1864,7 +1998,7 @@
       <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="43" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="8" t="s">
@@ -2178,13 +2312,13 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="40" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="47" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -2244,7 +2378,7 @@
       <c r="W18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="X18" s="8" t="s">
+      <c r="X18" s="28" t="s">
         <v>23</v>
       </c>
       <c r="Y18" s="10" t="s">
@@ -2362,10 +2496,10 @@
       <c r="G20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="30" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="8" t="s">
@@ -2493,7 +2627,7 @@
       <c r="W21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="X21" s="8" t="s">
+      <c r="X21" s="30" t="s">
         <v>23</v>
       </c>
       <c r="Y21" s="16" t="s">
@@ -2795,7 +2929,7 @@
       <c r="M25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N25" s="10" t="s">
+      <c r="N25" s="51" t="s">
         <v>39</v>
       </c>
       <c r="O25" s="8" t="s">
@@ -2845,7 +2979,7 @@
       <c r="B26" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="34" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="21" t="s">
@@ -2996,6 +3130,48 @@
       </c>
       <c r="Z27" s="3">
         <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B28" s="38"/>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="P28" s="45"/>
+      <c r="R28" s="48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B29" s="31"/>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="P29" s="44"/>
+      <c r="R29" s="49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B30" s="37"/>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="P30" s="50"/>
+      <c r="R30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B31" s="41"/>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B32" s="42"/>
+      <c r="D32" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>